<commit_message>
feat: hw4 excel done
</commit_message>
<xml_diff>
--- a/xlsx/hw4.xlsx
+++ b/xlsx/hw4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adithyah Nair\source\repos\xll_ml\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B378FB79-C9DC-40CE-9424-4BDAF186700D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C86C06-3752-4862-B3AD-D7295DB3FBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="3" xr2:uid="{EDEE3299-5466-402C-8B4F-6E69C4CA67FB}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>https://home.treasury.gov/resource-center/data-chart-center/interest-rates/daily-treasury-rates.csv/2026/all?field_tdr_date_value=2026&amp;type=daily_treasury_yield_curve&amp;page&amp;_format=csv</t>
   </si>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t>forward</t>
-  </si>
-  <si>
-    <t>insert graph</t>
   </si>
   <si>
     <t>plot curve here using pwflate.spot, forward</t>
@@ -403,6 +400,1828 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.9400481189851269E-2"/>
+          <c:y val="2.5428331875182269E-2"/>
+          <c:w val="0.86348840769903767"/>
+          <c:h val="0.6714577865266842"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Bootstrap!$K$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>spot</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Bootstrap!$I$6:$I$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="69"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>28.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Bootstrap!$K$6:$K$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="69"/>
+                <c:pt idx="0">
+                  <c:v>8.3460694718096292E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1721652552653194E-8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3426533629957488E-12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.3066525868486428E-15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1720659910274133E-15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1203443653368078E-17</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.182702832307702E-17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.0584696912845166E-17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5.2393490839786813E-17</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-7.7133663894074747E-17</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-9.6925802337505126E-17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.3341709923999684E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.5012564885999575E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.5076070258772928E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.511840717395516E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.5656493243924323E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.6060057796401188E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.6373941337216532E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.6625048169868814E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.7287617455359773E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.7839758526602242E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.830695481765356E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.870740878141183E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.9263487420600054E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.9750056229889752E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.0179381649851242E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.0561004245372574E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.0902456041365345E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.1209762657758831E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.1863573592166539E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.2457947168900806E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.3000636086788627E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.349810092818579E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.3955768582271189E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.4378231032196166E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.4769399967311892E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.5132628264205055E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.5470806333726278E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.5786439198612756E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.6081708652861396E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.6358523766219496E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.6618562206040749E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.6863304267048975E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.709406106742816E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.731199804556406E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.7518154646503434E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.7713460900024936E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7898751448237645E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8074777469039723E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.8101302154853053E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.8126563760389554E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.8150650407529007E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.817364220707121E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.8195612148855996E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.8216626875780558E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.8236747359006203E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.8256029488764125E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.8274524592817634E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.8292279892709011E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.8309338906330129E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.8325741804042741E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.8341525724483178E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.8356725055277688E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.8371371683134198E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.8385495217138703E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.8399123188546549E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.8412281229905853E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.8424993235964837E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.8437281508488535E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B686-4DC3-8740-FDF16732476B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Bootstrap!$L$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>forward</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Bootstrap!$I$6:$I$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="69"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.79999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>9.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>17.5</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>18.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>19.5</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>20.5</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>21.5</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>22.5</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>23.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>24.5</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>26.5</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>27.5</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>28.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>29.5</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Bootstrap!$L$6:$L$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="69"/>
+                <c:pt idx="0">
+                  <c:v>8.3460694718096292E-8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1.6697355827456216E-7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1.7442842526169745E-11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2389158665652486E-14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-4.2822467458428146E-15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-4.2822467458428146E-15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-2.7505504832837833E-16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.7505504832837833E-16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-2.7505504832837833E-16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-2.7505504832837833E-16</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-2.7505504832837833E-16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0025129771999248E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0025129771999248E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.533009174986633E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.533009174986633E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.8885009663739284E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.8885009663739284E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.8885009663739284E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.8885009663739284E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.3913310310269391E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4.3913310310269391E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.3913310310269391E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>4.3913310310269391E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.7048588369235173E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.7048588369235173E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.7048588369235173E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.7048588369235173E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.7048588369235173E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.7048588369235173E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.4939792280320608E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4.9162289587386152E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B686-4DC3-8740-FDF16732476B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="64113856"/>
+        <c:axId val="64114336"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="64113856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64114336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="64114336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64113856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>481012</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>566737</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1AF0C90-48EF-4ADB-9399-970166158C44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -724,7 +2543,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{643E00C4-F6CC-4E64-A377-FDB90E30013C}">
   <dimension ref="B2:P38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B17" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
@@ -2356,12 +4175,12 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -2369,7 +4188,7 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" cm="1">
         <f t="array" ref="C6">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C5)</f>
@@ -2378,7 +4197,7 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" cm="1">
         <f t="array" ref="C7:C8">_xll.FI.INSTRUMENT(C6)</f>
@@ -2392,12 +4211,12 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -2405,7 +4224,7 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11">
         <v>0.05</v>
@@ -2413,7 +4232,7 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -2421,7 +4240,7 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" cm="1">
         <f t="array" ref="C13">_xll.\FI.INSTRUMENT.BOND(C10,C11,C12)</f>
@@ -2430,7 +4249,7 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" cm="1">
         <f t="array" ref="C14:F15">_xll.FI.INSTRUMENT(C13)</f>
@@ -2488,7 +4307,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2502,7 +4321,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5">
         <v>0.03</v>
@@ -2516,7 +4335,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C6" cm="1">
         <f t="array" ref="C6">_xll.\FI.CURVE.PWFLAT(C4:E4,C5:E5)</f>
@@ -2525,7 +4344,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" cm="1">
         <f t="array" ref="C7:E8">_xll.FI.CURVE.PWFLAT(C6)</f>
@@ -2540,7 +4359,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8">
         <v>0.03</v>
@@ -2554,7 +4373,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" cm="1">
         <f t="array" ref="C9">_xll.FI.CURVE.FORWARD(C6,1)</f>
@@ -2563,7 +4382,7 @@
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" cm="1">
         <f t="array" ref="C10">_xll.FI.CURVE.DISCOUNT(C6,1)</f>
@@ -2585,13 +4404,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2E5B4B-30B9-4C78-A319-DEE69FDAA7AA}">
   <dimension ref="B2:L74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
@@ -2633,6 +4453,10 @@
         <f t="array" ref="F3">_xll.\FI.INSTRUMENT.ZERO_COUPON_BOND(C3,E3)</f>
         <v>2564535987280</v>
       </c>
+      <c r="G3" cm="1">
+        <f t="array" ref="G3">_xll.\FI.CURVE.PWFLAT.BOOTSTRAP(F3:F16,E3:E16)</f>
+        <v>2564535974176</v>
+      </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -2654,7 +4478,7 @@
         <v>2564539364064</v>
       </c>
       <c r="I4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
@@ -2679,10 +4503,11 @@
       <c r="I5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="7"/>
+      <c r="K5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="L5" s="7" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2712,6 +4537,14 @@
         <f t="array" ref="I6:I74">_xlfn.VSTACK(_xlfn.SEQUENCE(1/H6,1,0,H6),_xlfn.SEQUENCE(1+29/H7,1,1,H7))</f>
         <v>0</v>
       </c>
+      <c r="K6" cm="1">
+        <f t="array" ref="K6">_xll.FI.CURVE.SPOT($G$3,I6)</f>
+        <v>8.3460694718096292E-8</v>
+      </c>
+      <c r="L6" cm="1">
+        <f t="array" ref="L6">_xll.FI.CURVE.FORWARD($G$3,I6)</f>
+        <v>8.3460694718096292E-8</v>
+      </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
@@ -2738,6 +4571,14 @@
       <c r="I7">
         <v>0.1</v>
       </c>
+      <c r="K7" cm="1">
+        <f t="array" ref="K7">_xll.FI.CURVE.SPOT($G$3,I7)</f>
+        <v>4.1721652552653194E-8</v>
+      </c>
+      <c r="L7" cm="1">
+        <f t="array" ref="L7">_xll.FI.CURVE.FORWARD($G$3,I7)</f>
+        <v>-1.6697355827456216E-7</v>
+      </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -2761,6 +4602,14 @@
       <c r="I8">
         <v>0.2</v>
       </c>
+      <c r="K8" cm="1">
+        <f t="array" ref="K8">_xll.FI.CURVE.SPOT($G$3,I8)</f>
+        <v>4.3426533629957488E-12</v>
+      </c>
+      <c r="L8" cm="1">
+        <f t="array" ref="L8">_xll.FI.CURVE.FORWARD($G$3,I8)</f>
+        <v>-1.7442842526169745E-11</v>
+      </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
@@ -2783,8 +4632,13 @@
       <c r="I9">
         <v>0.30000000000000004</v>
       </c>
-      <c r="L9" s="6" t="s">
-        <v>26</v>
+      <c r="K9" cm="1">
+        <f t="array" ref="K9">_xll.FI.CURVE.SPOT($G$3,I9)</f>
+        <v>-3.3066525868486428E-15</v>
+      </c>
+      <c r="L9" cm="1">
+        <f t="array" ref="L9">_xll.FI.CURVE.FORWARD($G$3,I9)</f>
+        <v>5.2389158665652486E-14</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.3">
@@ -2807,6 +4661,14 @@
       <c r="I10">
         <v>0.4</v>
       </c>
+      <c r="K10" cm="1">
+        <f t="array" ref="K10">_xll.FI.CURVE.SPOT($G$3,I10)</f>
+        <v>1.1720659910274133E-15</v>
+      </c>
+      <c r="L10" cm="1">
+        <f t="array" ref="L10">_xll.FI.CURVE.FORWARD($G$3,I10)</f>
+        <v>-4.2822467458428146E-15</v>
+      </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -2828,6 +4690,14 @@
       <c r="I11">
         <v>0.5</v>
       </c>
+      <c r="K11" cm="1">
+        <f t="array" ref="K11">_xll.FI.CURVE.SPOT($G$3,I11)</f>
+        <v>8.1203443653368078E-17</v>
+      </c>
+      <c r="L11" cm="1">
+        <f t="array" ref="L11">_xll.FI.CURVE.FORWARD($G$3,I11)</f>
+        <v>-4.2822467458428146E-15</v>
+      </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
@@ -2849,6 +4719,14 @@
       <c r="I12">
         <v>0.6</v>
       </c>
+      <c r="K12" cm="1">
+        <f t="array" ref="K12">_xll.FI.CURVE.SPOT($G$3,I12)</f>
+        <v>2.182702832307702E-17</v>
+      </c>
+      <c r="L12" cm="1">
+        <f t="array" ref="L12">_xll.FI.CURVE.FORWARD($G$3,I12)</f>
+        <v>-2.7505504832837833E-16</v>
+      </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
@@ -2870,6 +4748,14 @@
       <c r="I13">
         <v>0.7</v>
       </c>
+      <c r="K13" cm="1">
+        <f t="array" ref="K13">_xll.FI.CURVE.SPOT($G$3,I13)</f>
+        <v>-2.0584696912845166E-17</v>
+      </c>
+      <c r="L13" cm="1">
+        <f t="array" ref="L13">_xll.FI.CURVE.FORWARD($G$3,I13)</f>
+        <v>-2.7505504832837833E-16</v>
+      </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
@@ -2891,6 +4777,14 @@
       <c r="I14">
         <v>0.79999999999999993</v>
       </c>
+      <c r="K14" cm="1">
+        <f t="array" ref="K14">_xll.FI.CURVE.SPOT($G$3,I14)</f>
+        <v>-5.2393490839786813E-17</v>
+      </c>
+      <c r="L14" cm="1">
+        <f t="array" ref="L14">_xll.FI.CURVE.FORWARD($G$3,I14)</f>
+        <v>-2.7505504832837833E-16</v>
+      </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -2912,6 +4806,14 @@
       <c r="I15">
         <v>0.89999999999999991</v>
       </c>
+      <c r="K15" cm="1">
+        <f t="array" ref="K15">_xll.FI.CURVE.SPOT($G$3,I15)</f>
+        <v>-7.7133663894074747E-17</v>
+      </c>
+      <c r="L15" cm="1">
+        <f t="array" ref="L15">_xll.FI.CURVE.FORWARD($G$3,I15)</f>
+        <v>-2.7505504832837833E-16</v>
+      </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
@@ -2933,295 +4835,767 @@
       <c r="I16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K16" cm="1">
+        <f t="array" ref="K16">_xll.FI.CURVE.SPOT($G$3,I16)</f>
+        <v>-9.6925802337505126E-17</v>
+      </c>
+      <c r="L16" cm="1">
+        <f t="array" ref="L16">_xll.FI.CURVE.FORWARD($G$3,I16)</f>
+        <v>-2.7505504832837833E-16</v>
+      </c>
+    </row>
+    <row r="17" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I17">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="18" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K17" cm="1">
+        <f t="array" ref="K17">_xll.FI.CURVE.SPOT($G$3,I17)</f>
+        <v>2.3341709923999684E-2</v>
+      </c>
+      <c r="L17" cm="1">
+        <f t="array" ref="L17">_xll.FI.CURVE.FORWARD($G$3,I17)</f>
+        <v>7.0025129771999248E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I18">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K18" cm="1">
+        <f t="array" ref="K18">_xll.FI.CURVE.SPOT($G$3,I18)</f>
+        <v>3.5012564885999575E-2</v>
+      </c>
+      <c r="L18" cm="1">
+        <f t="array" ref="L18">_xll.FI.CURVE.FORWARD($G$3,I18)</f>
+        <v>7.0025129771999248E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I19">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="20" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K19" cm="1">
+        <f t="array" ref="K19">_xll.FI.CURVE.SPOT($G$3,I19)</f>
+        <v>3.5076070258772928E-2</v>
+      </c>
+      <c r="L19" cm="1">
+        <f t="array" ref="L19">_xll.FI.CURVE.FORWARD($G$3,I19)</f>
+        <v>3.533009174986633E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I20">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K20" cm="1">
+        <f t="array" ref="K20">_xll.FI.CURVE.SPOT($G$3,I20)</f>
+        <v>3.511840717395516E-2</v>
+      </c>
+      <c r="L20" cm="1">
+        <f t="array" ref="L20">_xll.FI.CURVE.FORWARD($G$3,I20)</f>
+        <v>3.533009174986633E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I21">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="22" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K21" cm="1">
+        <f t="array" ref="K21">_xll.FI.CURVE.SPOT($G$3,I21)</f>
+        <v>3.5656493243924323E-2</v>
+      </c>
+      <c r="L21" cm="1">
+        <f t="array" ref="L21">_xll.FI.CURVE.FORWARD($G$3,I21)</f>
+        <v>3.8885009663739284E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K22" cm="1">
+        <f t="array" ref="K22">_xll.FI.CURVE.SPOT($G$3,I22)</f>
+        <v>3.6060057796401188E-2</v>
+      </c>
+      <c r="L22" cm="1">
+        <f t="array" ref="L22">_xll.FI.CURVE.FORWARD($G$3,I22)</f>
+        <v>3.8885009663739284E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I23">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="24" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K23" cm="1">
+        <f t="array" ref="K23">_xll.FI.CURVE.SPOT($G$3,I23)</f>
+        <v>3.6373941337216532E-2</v>
+      </c>
+      <c r="L23" cm="1">
+        <f t="array" ref="L23">_xll.FI.CURVE.FORWARD($G$3,I23)</f>
+        <v>3.8885009663739284E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K24" cm="1">
+        <f t="array" ref="K24">_xll.FI.CURVE.SPOT($G$3,I24)</f>
+        <v>3.6625048169868814E-2</v>
+      </c>
+      <c r="L24" cm="1">
+        <f t="array" ref="L24">_xll.FI.CURVE.FORWARD($G$3,I24)</f>
+        <v>3.8885009663739284E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I25">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="26" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K25" cm="1">
+        <f t="array" ref="K25">_xll.FI.CURVE.SPOT($G$3,I25)</f>
+        <v>3.7287617455359773E-2</v>
+      </c>
+      <c r="L25" cm="1">
+        <f t="array" ref="L25">_xll.FI.CURVE.FORWARD($G$3,I25)</f>
+        <v>4.3913310310269391E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K26" cm="1">
+        <f t="array" ref="K26">_xll.FI.CURVE.SPOT($G$3,I26)</f>
+        <v>3.7839758526602242E-2</v>
+      </c>
+      <c r="L26" cm="1">
+        <f t="array" ref="L26">_xll.FI.CURVE.FORWARD($G$3,I26)</f>
+        <v>4.3913310310269391E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I27">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="28" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K27" cm="1">
+        <f t="array" ref="K27">_xll.FI.CURVE.SPOT($G$3,I27)</f>
+        <v>3.830695481765356E-2</v>
+      </c>
+      <c r="L27" cm="1">
+        <f t="array" ref="L27">_xll.FI.CURVE.FORWARD($G$3,I27)</f>
+        <v>4.3913310310269391E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I28">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K28" cm="1">
+        <f t="array" ref="K28">_xll.FI.CURVE.SPOT($G$3,I28)</f>
+        <v>3.870740878141183E-2</v>
+      </c>
+      <c r="L28" cm="1">
+        <f t="array" ref="L28">_xll.FI.CURVE.FORWARD($G$3,I28)</f>
+        <v>4.3913310310269391E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I29">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="30" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K29" cm="1">
+        <f t="array" ref="K29">_xll.FI.CURVE.SPOT($G$3,I29)</f>
+        <v>3.9263487420600054E-2</v>
+      </c>
+      <c r="L29" cm="1">
+        <f t="array" ref="L29">_xll.FI.CURVE.FORWARD($G$3,I29)</f>
+        <v>4.7048588369235173E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I30">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K30" cm="1">
+        <f t="array" ref="K30">_xll.FI.CURVE.SPOT($G$3,I30)</f>
+        <v>3.9750056229889752E-2</v>
+      </c>
+      <c r="L30" cm="1">
+        <f t="array" ref="L30">_xll.FI.CURVE.FORWARD($G$3,I30)</f>
+        <v>4.7048588369235173E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I31">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="32" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K31" cm="1">
+        <f t="array" ref="K31">_xll.FI.CURVE.SPOT($G$3,I31)</f>
+        <v>4.0179381649851242E-2</v>
+      </c>
+      <c r="L31" cm="1">
+        <f t="array" ref="L31">_xll.FI.CURVE.FORWARD($G$3,I31)</f>
+        <v>4.7048588369235173E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I32">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K32" cm="1">
+        <f t="array" ref="K32">_xll.FI.CURVE.SPOT($G$3,I32)</f>
+        <v>4.0561004245372574E-2</v>
+      </c>
+      <c r="L32" cm="1">
+        <f t="array" ref="L32">_xll.FI.CURVE.FORWARD($G$3,I32)</f>
+        <v>4.7048588369235173E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I33">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="34" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K33" cm="1">
+        <f t="array" ref="K33">_xll.FI.CURVE.SPOT($G$3,I33)</f>
+        <v>4.0902456041365345E-2</v>
+      </c>
+      <c r="L33" cm="1">
+        <f t="array" ref="L33">_xll.FI.CURVE.FORWARD($G$3,I33)</f>
+        <v>4.7048588369235173E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I34">
         <v>10</v>
       </c>
-    </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K34" cm="1">
+        <f t="array" ref="K34">_xll.FI.CURVE.SPOT($G$3,I34)</f>
+        <v>4.1209762657758831E-2</v>
+      </c>
+      <c r="L34" cm="1">
+        <f t="array" ref="L34">_xll.FI.CURVE.FORWARD($G$3,I34)</f>
+        <v>4.7048588369235173E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I35">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K35" cm="1">
+        <f t="array" ref="K35">_xll.FI.CURVE.SPOT($G$3,I35)</f>
+        <v>4.1863573592166539E-2</v>
+      </c>
+      <c r="L35" cm="1">
+        <f t="array" ref="L35">_xll.FI.CURVE.FORWARD($G$3,I35)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I36">
         <v>11</v>
       </c>
-    </row>
-    <row r="37" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K36" cm="1">
+        <f t="array" ref="K36">_xll.FI.CURVE.SPOT($G$3,I36)</f>
+        <v>4.2457947168900806E-2</v>
+      </c>
+      <c r="L36" cm="1">
+        <f t="array" ref="L36">_xll.FI.CURVE.FORWARD($G$3,I36)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I37">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="38" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K37" cm="1">
+        <f t="array" ref="K37">_xll.FI.CURVE.SPOT($G$3,I37)</f>
+        <v>4.3000636086788627E-2</v>
+      </c>
+      <c r="L37" cm="1">
+        <f t="array" ref="L37">_xll.FI.CURVE.FORWARD($G$3,I37)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I38">
         <v>12</v>
       </c>
-    </row>
-    <row r="39" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K38" cm="1">
+        <f t="array" ref="K38">_xll.FI.CURVE.SPOT($G$3,I38)</f>
+        <v>4.349810092818579E-2</v>
+      </c>
+      <c r="L38" cm="1">
+        <f t="array" ref="L38">_xll.FI.CURVE.FORWARD($G$3,I38)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I39">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="40" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K39" cm="1">
+        <f t="array" ref="K39">_xll.FI.CURVE.SPOT($G$3,I39)</f>
+        <v>4.3955768582271189E-2</v>
+      </c>
+      <c r="L39" cm="1">
+        <f t="array" ref="L39">_xll.FI.CURVE.FORWARD($G$3,I39)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I40">
         <v>13</v>
       </c>
-    </row>
-    <row r="41" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K40" cm="1">
+        <f t="array" ref="K40">_xll.FI.CURVE.SPOT($G$3,I40)</f>
+        <v>4.4378231032196166E-2</v>
+      </c>
+      <c r="L40" cm="1">
+        <f t="array" ref="L40">_xll.FI.CURVE.FORWARD($G$3,I40)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I41">
         <v>13.5</v>
       </c>
-    </row>
-    <row r="42" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K41" cm="1">
+        <f t="array" ref="K41">_xll.FI.CURVE.SPOT($G$3,I41)</f>
+        <v>4.4769399967311892E-2</v>
+      </c>
+      <c r="L41" cm="1">
+        <f t="array" ref="L41">_xll.FI.CURVE.FORWARD($G$3,I41)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I42">
         <v>14</v>
       </c>
-    </row>
-    <row r="43" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K42" cm="1">
+        <f t="array" ref="K42">_xll.FI.CURVE.SPOT($G$3,I42)</f>
+        <v>4.5132628264205055E-2</v>
+      </c>
+      <c r="L42" cm="1">
+        <f t="array" ref="L42">_xll.FI.CURVE.FORWARD($G$3,I42)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I43">
         <v>14.5</v>
       </c>
-    </row>
-    <row r="44" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K43" cm="1">
+        <f t="array" ref="K43">_xll.FI.CURVE.SPOT($G$3,I43)</f>
+        <v>4.5470806333726278E-2</v>
+      </c>
+      <c r="L43" cm="1">
+        <f t="array" ref="L43">_xll.FI.CURVE.FORWARD($G$3,I43)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I44">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K44" cm="1">
+        <f t="array" ref="K44">_xll.FI.CURVE.SPOT($G$3,I44)</f>
+        <v>4.5786439198612756E-2</v>
+      </c>
+      <c r="L44" cm="1">
+        <f t="array" ref="L44">_xll.FI.CURVE.FORWARD($G$3,I44)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I45">
         <v>15.5</v>
       </c>
-    </row>
-    <row r="46" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K45" cm="1">
+        <f t="array" ref="K45">_xll.FI.CURVE.SPOT($G$3,I45)</f>
+        <v>4.6081708652861396E-2</v>
+      </c>
+      <c r="L45" cm="1">
+        <f t="array" ref="L45">_xll.FI.CURVE.FORWARD($G$3,I45)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I46">
         <v>16</v>
       </c>
-    </row>
-    <row r="47" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K46" cm="1">
+        <f t="array" ref="K46">_xll.FI.CURVE.SPOT($G$3,I46)</f>
+        <v>4.6358523766219496E-2</v>
+      </c>
+      <c r="L46" cm="1">
+        <f t="array" ref="L46">_xll.FI.CURVE.FORWARD($G$3,I46)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I47">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="48" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K47" cm="1">
+        <f t="array" ref="K47">_xll.FI.CURVE.SPOT($G$3,I47)</f>
+        <v>4.6618562206040749E-2</v>
+      </c>
+      <c r="L47" cm="1">
+        <f t="array" ref="L47">_xll.FI.CURVE.FORWARD($G$3,I47)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I48">
         <v>17</v>
       </c>
-    </row>
-    <row r="49" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K48" cm="1">
+        <f t="array" ref="K48">_xll.FI.CURVE.SPOT($G$3,I48)</f>
+        <v>4.6863304267048975E-2</v>
+      </c>
+      <c r="L48" cm="1">
+        <f t="array" ref="L48">_xll.FI.CURVE.FORWARD($G$3,I48)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I49">
         <v>17.5</v>
       </c>
-    </row>
-    <row r="50" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K49" cm="1">
+        <f t="array" ref="K49">_xll.FI.CURVE.SPOT($G$3,I49)</f>
+        <v>4.709406106742816E-2</v>
+      </c>
+      <c r="L49" cm="1">
+        <f t="array" ref="L49">_xll.FI.CURVE.FORWARD($G$3,I49)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I50">
         <v>18</v>
       </c>
-    </row>
-    <row r="51" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K50" cm="1">
+        <f t="array" ref="K50">_xll.FI.CURVE.SPOT($G$3,I50)</f>
+        <v>4.731199804556406E-2</v>
+      </c>
+      <c r="L50" cm="1">
+        <f t="array" ref="L50">_xll.FI.CURVE.FORWARD($G$3,I50)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I51">
         <v>18.5</v>
       </c>
-    </row>
-    <row r="52" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K51" cm="1">
+        <f t="array" ref="K51">_xll.FI.CURVE.SPOT($G$3,I51)</f>
+        <v>4.7518154646503434E-2</v>
+      </c>
+      <c r="L51" cm="1">
+        <f t="array" ref="L51">_xll.FI.CURVE.FORWARD($G$3,I51)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I52">
         <v>19</v>
       </c>
-    </row>
-    <row r="53" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K52" cm="1">
+        <f t="array" ref="K52">_xll.FI.CURVE.SPOT($G$3,I52)</f>
+        <v>4.7713460900024936E-2</v>
+      </c>
+      <c r="L52" cm="1">
+        <f t="array" ref="L52">_xll.FI.CURVE.FORWARD($G$3,I52)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I53">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="54" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K53" cm="1">
+        <f t="array" ref="K53">_xll.FI.CURVE.SPOT($G$3,I53)</f>
+        <v>4.7898751448237645E-2</v>
+      </c>
+      <c r="L53" cm="1">
+        <f t="array" ref="L53">_xll.FI.CURVE.FORWARD($G$3,I53)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I54">
         <v>20</v>
       </c>
-    </row>
-    <row r="55" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K54" cm="1">
+        <f t="array" ref="K54">_xll.FI.CURVE.SPOT($G$3,I54)</f>
+        <v>4.8074777469039723E-2</v>
+      </c>
+      <c r="L54" cm="1">
+        <f t="array" ref="L54">_xll.FI.CURVE.FORWARD($G$3,I54)</f>
+        <v>5.4939792280320608E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I55">
         <v>20.5</v>
       </c>
-    </row>
-    <row r="56" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K55" cm="1">
+        <f t="array" ref="K55">_xll.FI.CURVE.SPOT($G$3,I55)</f>
+        <v>4.8101302154853053E-2</v>
+      </c>
+      <c r="L55" cm="1">
+        <f t="array" ref="L55">_xll.FI.CURVE.FORWARD($G$3,I55)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I56">
         <v>21</v>
       </c>
-    </row>
-    <row r="57" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K56" cm="1">
+        <f t="array" ref="K56">_xll.FI.CURVE.SPOT($G$3,I56)</f>
+        <v>4.8126563760389554E-2</v>
+      </c>
+      <c r="L56" cm="1">
+        <f t="array" ref="L56">_xll.FI.CURVE.FORWARD($G$3,I56)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I57">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="58" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K57" cm="1">
+        <f t="array" ref="K57">_xll.FI.CURVE.SPOT($G$3,I57)</f>
+        <v>4.8150650407529007E-2</v>
+      </c>
+      <c r="L57" cm="1">
+        <f t="array" ref="L57">_xll.FI.CURVE.FORWARD($G$3,I57)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I58">
         <v>22</v>
       </c>
-    </row>
-    <row r="59" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K58" cm="1">
+        <f t="array" ref="K58">_xll.FI.CURVE.SPOT($G$3,I58)</f>
+        <v>4.817364220707121E-2</v>
+      </c>
+      <c r="L58" cm="1">
+        <f t="array" ref="L58">_xll.FI.CURVE.FORWARD($G$3,I58)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I59">
         <v>22.5</v>
       </c>
-    </row>
-    <row r="60" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K59" cm="1">
+        <f t="array" ref="K59">_xll.FI.CURVE.SPOT($G$3,I59)</f>
+        <v>4.8195612148855996E-2</v>
+      </c>
+      <c r="L59" cm="1">
+        <f t="array" ref="L59">_xll.FI.CURVE.FORWARD($G$3,I59)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I60">
         <v>23</v>
       </c>
-    </row>
-    <row r="61" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K60" cm="1">
+        <f t="array" ref="K60">_xll.FI.CURVE.SPOT($G$3,I60)</f>
+        <v>4.8216626875780558E-2</v>
+      </c>
+      <c r="L60" cm="1">
+        <f t="array" ref="L60">_xll.FI.CURVE.FORWARD($G$3,I60)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I61">
         <v>23.5</v>
       </c>
-    </row>
-    <row r="62" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K61" cm="1">
+        <f t="array" ref="K61">_xll.FI.CURVE.SPOT($G$3,I61)</f>
+        <v>4.8236747359006203E-2</v>
+      </c>
+      <c r="L61" cm="1">
+        <f t="array" ref="L61">_xll.FI.CURVE.FORWARD($G$3,I61)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I62">
         <v>24</v>
       </c>
-    </row>
-    <row r="63" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K62" cm="1">
+        <f t="array" ref="K62">_xll.FI.CURVE.SPOT($G$3,I62)</f>
+        <v>4.8256029488764125E-2</v>
+      </c>
+      <c r="L62" cm="1">
+        <f t="array" ref="L62">_xll.FI.CURVE.FORWARD($G$3,I62)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I63">
         <v>24.5</v>
       </c>
-    </row>
-    <row r="64" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K63" cm="1">
+        <f t="array" ref="K63">_xll.FI.CURVE.SPOT($G$3,I63)</f>
+        <v>4.8274524592817634E-2</v>
+      </c>
+      <c r="L63" cm="1">
+        <f t="array" ref="L63">_xll.FI.CURVE.FORWARD($G$3,I63)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I64">
         <v>25</v>
       </c>
-    </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K64" cm="1">
+        <f t="array" ref="K64">_xll.FI.CURVE.SPOT($G$3,I64)</f>
+        <v>4.8292279892709011E-2</v>
+      </c>
+      <c r="L64" cm="1">
+        <f t="array" ref="L64">_xll.FI.CURVE.FORWARD($G$3,I64)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I65">
         <v>25.5</v>
       </c>
-    </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K65" cm="1">
+        <f t="array" ref="K65">_xll.FI.CURVE.SPOT($G$3,I65)</f>
+        <v>4.8309338906330129E-2</v>
+      </c>
+      <c r="L65" cm="1">
+        <f t="array" ref="L65">_xll.FI.CURVE.FORWARD($G$3,I65)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I66">
         <v>26</v>
       </c>
-    </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K66" cm="1">
+        <f t="array" ref="K66">_xll.FI.CURVE.SPOT($G$3,I66)</f>
+        <v>4.8325741804042741E-2</v>
+      </c>
+      <c r="L66" cm="1">
+        <f t="array" ref="L66">_xll.FI.CURVE.FORWARD($G$3,I66)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I67">
         <v>26.5</v>
       </c>
-    </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K67" cm="1">
+        <f t="array" ref="K67">_xll.FI.CURVE.SPOT($G$3,I67)</f>
+        <v>4.8341525724483178E-2</v>
+      </c>
+      <c r="L67" cm="1">
+        <f t="array" ref="L67">_xll.FI.CURVE.FORWARD($G$3,I67)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I68">
         <v>27</v>
       </c>
-    </row>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K68" cm="1">
+        <f t="array" ref="K68">_xll.FI.CURVE.SPOT($G$3,I68)</f>
+        <v>4.8356725055277688E-2</v>
+      </c>
+      <c r="L68" cm="1">
+        <f t="array" ref="L68">_xll.FI.CURVE.FORWARD($G$3,I68)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I69">
         <v>27.5</v>
       </c>
-    </row>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K69" cm="1">
+        <f t="array" ref="K69">_xll.FI.CURVE.SPOT($G$3,I69)</f>
+        <v>4.8371371683134198E-2</v>
+      </c>
+      <c r="L69" cm="1">
+        <f t="array" ref="L69">_xll.FI.CURVE.FORWARD($G$3,I69)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I70">
         <v>28</v>
       </c>
-    </row>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K70" cm="1">
+        <f t="array" ref="K70">_xll.FI.CURVE.SPOT($G$3,I70)</f>
+        <v>4.8385495217138703E-2</v>
+      </c>
+      <c r="L70" cm="1">
+        <f t="array" ref="L70">_xll.FI.CURVE.FORWARD($G$3,I70)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I71">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K71" cm="1">
+        <f t="array" ref="K71">_xll.FI.CURVE.SPOT($G$3,I71)</f>
+        <v>4.8399123188546549E-2</v>
+      </c>
+      <c r="L71" cm="1">
+        <f t="array" ref="L71">_xll.FI.CURVE.FORWARD($G$3,I71)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I72">
         <v>29</v>
       </c>
-    </row>
-    <row r="73" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K72" cm="1">
+        <f t="array" ref="K72">_xll.FI.CURVE.SPOT($G$3,I72)</f>
+        <v>4.8412281229905853E-2</v>
+      </c>
+      <c r="L72" cm="1">
+        <f t="array" ref="L72">_xll.FI.CURVE.FORWARD($G$3,I72)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I73">
         <v>29.5</v>
       </c>
-    </row>
-    <row r="74" spans="9:9" x14ac:dyDescent="0.3">
+      <c r="K73" cm="1">
+        <f t="array" ref="K73">_xll.FI.CURVE.SPOT($G$3,I73)</f>
+        <v>4.8424993235964837E-2</v>
+      </c>
+      <c r="L73" cm="1">
+        <f t="array" ref="L73">_xll.FI.CURVE.FORWARD($G$3,I73)</f>
+        <v>4.9162289587386152E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I74">
         <v>30</v>
+      </c>
+      <c r="K74" cm="1">
+        <f t="array" ref="K74">_xll.FI.CURVE.SPOT($G$3,I74)</f>
+        <v>4.8437281508488535E-2</v>
+      </c>
+      <c r="L74" cm="1">
+        <f t="array" ref="L74">_xll.FI.CURVE.FORWARD($G$3,I74)</f>
+        <v>4.9162289587386152E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3229,6 +5603,7 @@
   <ignoredErrors>
     <ignoredError sqref="C4" formula="1"/>
   </ignoredErrors>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>